<commit_message>
added grayed out punctuation marks.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0BA97B-9C21-4C35-A69B-4EE4D6CAFF91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA381FFC-DE3F-4D16-87D9-704732E96273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="573">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3020,18 +3020,12 @@
     <t>sit</t>
   </si>
   <si>
-    <t>amet,</t>
-  </si>
-  <si>
     <t>consectetur</t>
   </si>
   <si>
     <t>adipiscing</t>
   </si>
   <si>
-    <t>elit.</t>
-  </si>
-  <si>
     <t>Phasellus</t>
   </si>
   <si>
@@ -3041,9 +3035,6 @@
     <t>tortor</t>
   </si>
   <si>
-    <t>neque.</t>
-  </si>
-  <si>
     <t>Nulla</t>
   </si>
   <si>
@@ -3053,18 +3044,12 @@
     <t>dictum</t>
   </si>
   <si>
-    <t>nibh,</t>
-  </si>
-  <si>
     <t>eu</t>
   </si>
   <si>
     <t>vehicula</t>
   </si>
   <si>
-    <t>felis.</t>
-  </si>
-  <si>
     <t>Suspendisse</t>
   </si>
   <si>
@@ -3080,9 +3065,6 @@
     <t>viverra</t>
   </si>
   <si>
-    <t>fermentum.</t>
-  </si>
-  <si>
     <t>Ut</t>
   </si>
   <si>
@@ -3098,33 +3080,21 @@
     <t>rhoncus</t>
   </si>
   <si>
-    <t>suscipit.</t>
-  </si>
-  <si>
     <t>sed</t>
   </si>
   <si>
     <t>lacus</t>
   </si>
   <si>
-    <t>egestas,</t>
-  </si>
-  <si>
     <t>aliquam</t>
   </si>
   <si>
     <t>urna</t>
   </si>
   <si>
-    <t>eu,</t>
-  </si>
-  <si>
     <t>sollicitudin</t>
   </si>
   <si>
-    <t>risus.</t>
-  </si>
-  <si>
     <t>Vestibulum</t>
   </si>
   <si>
@@ -3134,9 +3104,6 @@
     <t>bibendum</t>
   </si>
   <si>
-    <t>imperdiet.</t>
-  </si>
-  <si>
     <t>Quisque</t>
   </si>
   <si>
@@ -3146,39 +3113,24 @@
     <t>felis</t>
   </si>
   <si>
-    <t>tellus.</t>
-  </si>
-  <si>
     <t>Vivamus</t>
   </si>
   <si>
     <t>amet</t>
   </si>
   <si>
-    <t>diam,</t>
-  </si>
-  <si>
     <t>eget</t>
   </si>
   <si>
     <t>auctor</t>
   </si>
   <si>
-    <t>ligula.</t>
-  </si>
-  <si>
-    <t>vestibulum,</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>pharetra</t>
   </si>
   <si>
-    <t>iaculis,</t>
-  </si>
-  <si>
     <t>mi</t>
   </si>
   <si>
@@ -3188,9 +3140,6 @@
     <t>tristique</t>
   </si>
   <si>
-    <t>urna,</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
@@ -3215,9 +3164,6 @@
     <t>erat</t>
   </si>
   <si>
-    <t>feugiat.</t>
-  </si>
-  <si>
     <t>Nullam</t>
   </si>
   <si>
@@ -3227,9 +3173,6 @@
     <t>mattis</t>
   </si>
   <si>
-    <t>metus,</t>
-  </si>
-  <si>
     <t>fringilla</t>
   </si>
   <si>
@@ -3239,9 +3182,6 @@
     <t>pulvinar</t>
   </si>
   <si>
-    <t>a.</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -3249,6 +3189,42 @@
   </si>
   <si>
     <t>custom-egra-grid(type='reading', duration='30')</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>tellus</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>diam</t>
+  </si>
+  <si>
+    <t>ligula</t>
+  </si>
+  <si>
+    <t>feugiat</t>
+  </si>
+  <si>
+    <t>elit</t>
+  </si>
+  <si>
+    <t>neque</t>
+  </si>
+  <si>
+    <t>fermentum</t>
+  </si>
+  <si>
+    <t>suscipit</t>
+  </si>
+  <si>
+    <t>egestas</t>
+  </si>
+  <si>
+    <t>iaculis</t>
   </si>
 </sst>
 </file>
@@ -3957,7 +3933,23 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="231">
+  <dxfs count="232">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6131,8 +6123,8 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -6346,7 +6338,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="9" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>361</v>
@@ -6358,7 +6350,7 @@
         <v>381</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -6371,9 +6363,6 @@
       <c r="C14" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="D14" s="11">
-        <v>14</v>
-      </c>
       <c r="N14" s="9" t="s">
         <v>373</v>
       </c>
@@ -6388,9 +6377,6 @@
       <c r="C15" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="D15" s="11">
-        <v>13</v>
-      </c>
       <c r="N15" s="9" t="s">
         <v>374</v>
       </c>
@@ -6405,9 +6391,6 @@
       <c r="C16" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="D16" s="11">
-        <v>12</v>
-      </c>
       <c r="N16" s="9" t="s">
         <v>375</v>
       </c>
@@ -6422,9 +6405,6 @@
       <c r="C17" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="D17" s="11">
-        <v>11</v>
-      </c>
       <c r="N17" s="9" t="s">
         <v>376</v>
       </c>
@@ -6471,7 +6451,7 @@
         <v>496</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -6485,7 +6465,7 @@
         <v>368</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N21" s="9" t="s">
         <v>373</v>
@@ -6502,7 +6482,7 @@
         <v>369</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N22" s="9" t="s">
         <v>374</v>
@@ -6518,8 +6498,11 @@
       <c r="C23" s="10" t="s">
         <v>370</v>
       </c>
+      <c r="D23" s="11">
+        <v>12</v>
+      </c>
       <c r="J23" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N23" s="9" t="s">
         <v>375</v>
@@ -6536,7 +6519,7 @@
         <v>371</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N24" s="9" t="s">
         <v>376</v>
@@ -6553,7 +6536,7 @@
         <v>372</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N25" s="9" t="s">
         <v>377</v>
@@ -6570,7 +6553,7 @@
         <v>494</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -6590,7 +6573,7 @@
         <v>486</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -6604,7 +6587,7 @@
         <v>368</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N28" s="9" t="s">
         <v>481</v>
@@ -6621,7 +6604,7 @@
         <v>369</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N29" s="9" t="s">
         <v>482</v>
@@ -6638,7 +6621,7 @@
         <v>370</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N30" s="9" t="s">
         <v>483</v>
@@ -6655,7 +6638,7 @@
         <v>371</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N31" s="9" t="s">
         <v>484</v>
@@ -6672,7 +6655,7 @@
         <v>372</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="N32" s="9" t="s">
         <v>485</v>
@@ -6689,517 +6672,517 @@
         <v>480</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:C19 I1:I19 F1:F19 F34:F1048576 I34:I1048576 B34:C1048576">
-    <cfRule type="expression" dxfId="230" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="231" priority="146" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C19 O1:O19 I1:I19 I34:I1048576 O34:O1048576 B34:C1048576">
-    <cfRule type="expression" dxfId="229" priority="143" stopIfTrue="1">
+    <cfRule type="expression" dxfId="230" priority="143" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D19 F1:F19 F34:F1048576 B34:D1048576">
-    <cfRule type="expression" dxfId="228" priority="140" stopIfTrue="1">
+    <cfRule type="expression" dxfId="229" priority="140" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D19 G1:H19 G34:H1048576 B34:D1048576">
-    <cfRule type="expression" dxfId="227" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="228" priority="138" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D19 G1:H19 G34:H1048576 B34:D1048576">
-    <cfRule type="expression" dxfId="226" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="227" priority="136" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C19 F1:F19 F34:F1048576 B34:C1048576">
-    <cfRule type="expression" dxfId="225" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="226" priority="131" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F19 B1:B19 B34:B1048576 F34:F1048576">
-    <cfRule type="expression" dxfId="224" priority="121" stopIfTrue="1">
+    <cfRule type="expression" dxfId="225" priority="121" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C19 B34:C1048576">
-    <cfRule type="expression" dxfId="223" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="224" priority="115" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="223" priority="117" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="119" stopIfTrue="1">
+    <cfRule type="expression" dxfId="222" priority="119" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B19 N1:N19 N34:N1048576 B34:B1048576">
-    <cfRule type="expression" dxfId="220" priority="113" stopIfTrue="1">
+    <cfRule type="expression" dxfId="221" priority="113" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C19 F1:F19 F34:F1048576 B34:C1048576">
-    <cfRule type="expression" dxfId="219" priority="111" stopIfTrue="1">
+    <cfRule type="expression" dxfId="220" priority="111" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C19 F1:F19 F34:F1048576 B34:C1048576">
-    <cfRule type="expression" dxfId="218" priority="107" stopIfTrue="1">
+    <cfRule type="expression" dxfId="219" priority="107" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C19 B34:C1048576">
-    <cfRule type="expression" dxfId="217" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="218" priority="105" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:W19 A34:W1048576">
-    <cfRule type="expression" dxfId="216" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="217" priority="102" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="215" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="106" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="215" priority="108" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="112" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="114" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="116" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="211" priority="118" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="120" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="209" priority="122" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="207" priority="125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="125" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="207" priority="132" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="137" stopIfTrue="1">
+    <cfRule type="expression" dxfId="206" priority="137" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="139" stopIfTrue="1">
+    <cfRule type="expression" dxfId="205" priority="139" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="141" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="141" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="142" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="144" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="145" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="147" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B19 B34:B1048576">
-    <cfRule type="expression" dxfId="198" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="100" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F33 I28:I33 B28:C33">
-    <cfRule type="expression" dxfId="197" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="98" stopIfTrue="1">
       <formula>$A28="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I33 O28:O33 B28:C33">
-    <cfRule type="expression" dxfId="196" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="197" priority="95" stopIfTrue="1">
       <formula>$A28="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F33 B28:D33">
-    <cfRule type="expression" dxfId="195" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="196" priority="92" stopIfTrue="1">
       <formula>$A28="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:H33 B28:D33">
-    <cfRule type="expression" dxfId="194" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="195" priority="90" stopIfTrue="1">
       <formula>$A28="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:H33 B28:D33">
-    <cfRule type="expression" dxfId="193" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="88" stopIfTrue="1">
       <formula>$A28="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F33 B28:C33">
-    <cfRule type="expression" dxfId="192" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="193" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A28, 16)="select_multiple ", LEN($A28)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A28, 17)))), AND(LEFT($A28, 11)="select_one ", LEN($A28)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A28, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B33 F28:F33">
-    <cfRule type="expression" dxfId="191" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="192" priority="83" stopIfTrue="1">
       <formula>OR($A28="audio audit", $A28="text audit", $A28="speed violations count", $A28="speed violations list", $A28="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:C33">
-    <cfRule type="expression" dxfId="190" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="191" priority="77" stopIfTrue="1">
       <formula>$A28="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="190" priority="79" stopIfTrue="1">
       <formula>$A28="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="189" priority="81" stopIfTrue="1">
       <formula>OR($A28="geopoint", $A28="geoshape", $A28="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28:N33 B28:B33">
-    <cfRule type="expression" dxfId="187" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="75" stopIfTrue="1">
       <formula>OR($A28="calculate", $A28="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F33 B28:C33">
-    <cfRule type="expression" dxfId="186" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="73" stopIfTrue="1">
       <formula>OR($A28="date", $A28="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F33 B28:C33">
-    <cfRule type="expression" dxfId="185" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="71" stopIfTrue="1">
       <formula>$A28="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:C33">
-    <cfRule type="expression" dxfId="184" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="69" stopIfTrue="1">
       <formula>OR($A28="audio", $A28="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:I33 K28:W33">
-    <cfRule type="expression" dxfId="183" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="68" stopIfTrue="1">
       <formula>$A28="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="70" stopIfTrue="1">
       <formula>OR($A28="audio", $A28="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="72" stopIfTrue="1">
       <formula>$A28="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="74" stopIfTrue="1">
       <formula>OR($A28="date", $A28="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="76" stopIfTrue="1">
       <formula>OR($A28="calculate", $A28="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="78" stopIfTrue="1">
       <formula>$A28="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="80" stopIfTrue="1">
       <formula>$A28="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="82" stopIfTrue="1">
       <formula>OR($A28="geopoint", $A28="geoshape", $A28="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="84" stopIfTrue="1">
       <formula>OR($A28="audio audit", $A28="text audit", $A28="speed violations count", $A28="speed violations list", $A28="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="85" stopIfTrue="1">
       <formula>OR($A28="username", $A28="phonenumber", $A28="start", $A28="end", $A28="deviceid", $A28="subscriberid", $A28="simserial", $A28="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="87" stopIfTrue="1">
       <formula>OR(AND(LEFT($A28, 16)="select_multiple ", LEN($A28)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A28, 17)))), AND(LEFT($A28, 11)="select_one ", LEN($A28)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A28, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="89" stopIfTrue="1">
       <formula>$A28="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="91" stopIfTrue="1">
       <formula>$A28="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="93" stopIfTrue="1">
       <formula>$A28="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="94" stopIfTrue="1">
       <formula>$A28="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="96" stopIfTrue="1">
       <formula>$A28="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="97" stopIfTrue="1">
       <formula>$A28="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="99" stopIfTrue="1">
       <formula>$A28="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B33">
-    <cfRule type="expression" dxfId="165" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="67" stopIfTrue="1">
       <formula>$A28="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C26 I20:I26 F20:F26">
-    <cfRule type="expression" dxfId="164" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="65" stopIfTrue="1">
       <formula>$A20="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C26 O20:O26 I20:I26">
-    <cfRule type="expression" dxfId="163" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="62" stopIfTrue="1">
       <formula>$A20="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:D26 F20:F26">
-    <cfRule type="expression" dxfId="162" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="59" stopIfTrue="1">
       <formula>$A20="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:D26 G20:H26">
-    <cfRule type="expression" dxfId="161" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="57" stopIfTrue="1">
       <formula>$A20="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:D26 G20:H26">
-    <cfRule type="expression" dxfId="160" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="55" stopIfTrue="1">
       <formula>$A20="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C26 F20:F26">
-    <cfRule type="expression" dxfId="159" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="53" stopIfTrue="1">
       <formula>OR(AND(LEFT($A20, 16)="select_multiple ", LEN($A20)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A20, 17)))), AND(LEFT($A20, 11)="select_one ", LEN($A20)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A20, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F26 B20:B26">
-    <cfRule type="expression" dxfId="158" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="50" stopIfTrue="1">
       <formula>OR($A20="audio audit", $A20="text audit", $A20="speed violations count", $A20="speed violations list", $A20="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C26">
-    <cfRule type="expression" dxfId="157" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="44" stopIfTrue="1">
       <formula>$A20="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="46" stopIfTrue="1">
       <formula>$A20="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="48" stopIfTrue="1">
       <formula>OR($A20="geopoint", $A20="geoshape", $A20="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B26 N20:N26">
-    <cfRule type="expression" dxfId="154" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="42" stopIfTrue="1">
       <formula>OR($A20="calculate", $A20="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C26 F20:F26">
-    <cfRule type="expression" dxfId="153" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="40" stopIfTrue="1">
       <formula>OR($A20="date", $A20="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C26 F20:F26">
-    <cfRule type="expression" dxfId="152" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="38" stopIfTrue="1">
       <formula>$A20="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C26">
-    <cfRule type="expression" dxfId="151" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="36" stopIfTrue="1">
       <formula>OR($A20="audio", $A20="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:W20 A21:I26 K21:W26 J21:J33">
-    <cfRule type="expression" dxfId="150" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="35" stopIfTrue="1">
       <formula>$A20="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="37" stopIfTrue="1">
       <formula>OR($A20="audio", $A20="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="39" stopIfTrue="1">
       <formula>$A20="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="41" stopIfTrue="1">
       <formula>OR($A20="date", $A20="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="43" stopIfTrue="1">
       <formula>OR($A20="calculate", $A20="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="45" stopIfTrue="1">
       <formula>$A20="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="47" stopIfTrue="1">
       <formula>$A20="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="49" stopIfTrue="1">
       <formula>OR($A20="geopoint", $A20="geoshape", $A20="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="51" stopIfTrue="1">
       <formula>OR($A20="audio audit", $A20="text audit", $A20="speed violations count", $A20="speed violations list", $A20="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="52" stopIfTrue="1">
       <formula>OR($A20="username", $A20="phonenumber", $A20="start", $A20="end", $A20="deviceid", $A20="subscriberid", $A20="simserial", $A20="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="54" stopIfTrue="1">
       <formula>OR(AND(LEFT($A20, 16)="select_multiple ", LEN($A20)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A20, 17)))), AND(LEFT($A20, 11)="select_one ", LEN($A20)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A20, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="56" stopIfTrue="1">
       <formula>$A20="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="58" stopIfTrue="1">
       <formula>$A20="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="60" stopIfTrue="1">
       <formula>$A20="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="61" stopIfTrue="1">
       <formula>$A20="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="63" stopIfTrue="1">
       <formula>$A20="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="64" stopIfTrue="1">
       <formula>$A20="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="66" stopIfTrue="1">
       <formula>$A20="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B26">
-    <cfRule type="expression" dxfId="132" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="34" stopIfTrue="1">
       <formula>$A20="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27 I27 F27">
-    <cfRule type="expression" dxfId="131" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="32" stopIfTrue="1">
       <formula>$A27="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27 O27 I27">
-    <cfRule type="expression" dxfId="130" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="29" stopIfTrue="1">
       <formula>$A27="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:D27 F27">
-    <cfRule type="expression" dxfId="129" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="26" stopIfTrue="1">
       <formula>$A27="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:D27 G27:H27">
-    <cfRule type="expression" dxfId="128" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="24" stopIfTrue="1">
       <formula>$A27="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:D27 G27:H27">
-    <cfRule type="expression" dxfId="127" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="22" stopIfTrue="1">
       <formula>$A27="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27 F27">
-    <cfRule type="expression" dxfId="126" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="20" stopIfTrue="1">
       <formula>OR(AND(LEFT($A27, 16)="select_multiple ", LEN($A27)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A27, 17)))), AND(LEFT($A27, 11)="select_one ", LEN($A27)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A27, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27 B27">
-    <cfRule type="expression" dxfId="125" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="17" stopIfTrue="1">
       <formula>OR($A27="audio audit", $A27="text audit", $A27="speed violations count", $A27="speed violations list", $A27="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27">
-    <cfRule type="expression" dxfId="124" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="11" stopIfTrue="1">
       <formula>$A27="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="13" stopIfTrue="1">
       <formula>$A27="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="15" stopIfTrue="1">
       <formula>OR($A27="geopoint", $A27="geoshape", $A27="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27 N27">
-    <cfRule type="expression" dxfId="121" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="9" stopIfTrue="1">
       <formula>OR($A27="calculate", $A27="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27 F27">
-    <cfRule type="expression" dxfId="120" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="7" stopIfTrue="1">
       <formula>OR($A27="date", $A27="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27 F27">
-    <cfRule type="expression" dxfId="119" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="5" stopIfTrue="1">
       <formula>$A27="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27">
-    <cfRule type="expression" dxfId="118" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="3" stopIfTrue="1">
       <formula>OR($A27="audio", $A27="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:I27 K27:W27">
-    <cfRule type="expression" dxfId="117" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="2" stopIfTrue="1">
       <formula>$A27="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="4" stopIfTrue="1">
       <formula>OR($A27="audio", $A27="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="6" stopIfTrue="1">
       <formula>$A27="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="8" stopIfTrue="1">
       <formula>OR($A27="date", $A27="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="10" stopIfTrue="1">
       <formula>OR($A27="calculate", $A27="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="12" stopIfTrue="1">
       <formula>$A27="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="14" stopIfTrue="1">
       <formula>$A27="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="16" stopIfTrue="1">
       <formula>OR($A27="geopoint", $A27="geoshape", $A27="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="18" stopIfTrue="1">
       <formula>OR($A27="audio audit", $A27="text audit", $A27="speed violations count", $A27="speed violations list", $A27="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="19" stopIfTrue="1">
       <formula>OR($A27="username", $A27="phonenumber", $A27="start", $A27="end", $A27="deviceid", $A27="subscriberid", $A27="simserial", $A27="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="21" stopIfTrue="1">
       <formula>OR(AND(LEFT($A27, 16)="select_multiple ", LEN($A27)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A27, 17)))), AND(LEFT($A27, 11)="select_one ", LEN($A27)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A27, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="23" stopIfTrue="1">
       <formula>$A27="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="25" stopIfTrue="1">
       <formula>$A27="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="27" stopIfTrue="1">
       <formula>$A27="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="28" stopIfTrue="1">
       <formula>$A27="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="30" stopIfTrue="1">
       <formula>$A27="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="31" stopIfTrue="1">
       <formula>$A27="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="33" stopIfTrue="1">
       <formula>$A27="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
       <formula>$A27="comments"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7211,11 +7194,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A157" sqref="A157:A244"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C238" sqref="C238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
@@ -8971,7 +8954,7 @@
         <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>504</v>
+        <v>536</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -8982,7 +8965,7 @@
         <v>6</v>
       </c>
       <c r="C162" t="s">
-        <v>505</v>
+        <v>563</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -8993,7 +8976,7 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -9004,7 +8987,7 @@
         <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -9015,7 +8998,7 @@
         <v>9</v>
       </c>
       <c r="C165" t="s">
-        <v>508</v>
+        <v>567</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -9026,7 +9009,7 @@
         <v>10</v>
       </c>
       <c r="C166" t="s">
-        <v>509</v>
+        <v>561</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -9037,7 +9020,7 @@
         <v>11</v>
       </c>
       <c r="C167" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -9048,7 +9031,7 @@
         <v>12</v>
       </c>
       <c r="C168" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -9059,7 +9042,7 @@
         <v>13</v>
       </c>
       <c r="C169" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -9070,7 +9053,7 @@
         <v>14</v>
       </c>
       <c r="C170" t="s">
-        <v>513</v>
+        <v>568</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -9081,7 +9064,7 @@
         <v>15</v>
       </c>
       <c r="C171" t="s">
-        <v>514</v>
+        <v>561</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -9092,7 +9075,7 @@
         <v>16</v>
       </c>
       <c r="C172" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -9103,7 +9086,7 @@
         <v>17</v>
       </c>
       <c r="C173" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -9114,7 +9097,7 @@
         <v>18</v>
       </c>
       <c r="C174" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -9125,7 +9108,7 @@
         <v>19</v>
       </c>
       <c r="C175" t="s">
-        <v>518</v>
+        <v>542</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -9136,7 +9119,7 @@
         <v>20</v>
       </c>
       <c r="C176" t="s">
-        <v>519</v>
+        <v>563</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -9147,7 +9130,7 @@
         <v>21</v>
       </c>
       <c r="C177" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -9158,7 +9141,7 @@
         <v>22</v>
       </c>
       <c r="C178" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -9169,7 +9152,7 @@
         <v>23</v>
       </c>
       <c r="C179" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -9180,7 +9163,7 @@
         <v>24</v>
       </c>
       <c r="C180" t="s">
-        <v>523</v>
+        <v>561</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -9191,7 +9174,7 @@
         <v>25</v>
       </c>
       <c r="C181" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -9202,7 +9185,7 @@
         <v>26</v>
       </c>
       <c r="C182" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -9213,7 +9196,7 @@
         <v>27</v>
       </c>
       <c r="C183" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -9224,7 +9207,7 @@
         <v>28</v>
       </c>
       <c r="C184" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -9235,7 +9218,7 @@
         <v>29</v>
       </c>
       <c r="C185" t="s">
-        <v>396</v>
+        <v>518</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -9246,7 +9229,7 @@
         <v>30</v>
       </c>
       <c r="C186" t="s">
-        <v>528</v>
+        <v>569</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -9257,7 +9240,7 @@
         <v>31</v>
       </c>
       <c r="C187" t="s">
-        <v>529</v>
+        <v>561</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -9268,7 +9251,7 @@
         <v>32</v>
       </c>
       <c r="C188" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -9279,7 +9262,7 @@
         <v>33</v>
       </c>
       <c r="C189" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -9290,7 +9273,7 @@
         <v>34</v>
       </c>
       <c r="C190" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -9301,7 +9284,7 @@
         <v>35</v>
       </c>
       <c r="C191" t="s">
-        <v>532</v>
+        <v>396</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -9312,7 +9295,7 @@
         <v>36</v>
       </c>
       <c r="C192" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -9323,7 +9306,7 @@
         <v>37</v>
       </c>
       <c r="C193" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -9334,7 +9317,7 @@
         <v>38</v>
       </c>
       <c r="C194" t="s">
-        <v>535</v>
+        <v>570</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -9345,7 +9328,7 @@
         <v>39</v>
       </c>
       <c r="C195" t="s">
-        <v>536</v>
+        <v>561</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -9356,7 +9339,7 @@
         <v>40</v>
       </c>
       <c r="C196" t="s">
-        <v>537</v>
+        <v>519</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -9367,7 +9350,7 @@
         <v>41</v>
       </c>
       <c r="C197" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -9378,7 +9361,7 @@
         <v>42</v>
       </c>
       <c r="C198" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -9389,7 +9372,7 @@
         <v>43</v>
       </c>
       <c r="C199" t="s">
-        <v>540</v>
+        <v>571</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -9400,7 +9383,7 @@
         <v>44</v>
       </c>
       <c r="C200" t="s">
-        <v>541</v>
+        <v>563</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -9411,7 +9394,7 @@
         <v>45</v>
       </c>
       <c r="C201" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -9422,7 +9405,7 @@
         <v>46</v>
       </c>
       <c r="C202" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -9433,7 +9416,7 @@
         <v>47</v>
       </c>
       <c r="C203" t="s">
-        <v>544</v>
+        <v>512</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -9444,7 +9427,7 @@
         <v>48</v>
       </c>
       <c r="C204" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -9455,7 +9438,7 @@
         <v>49</v>
       </c>
       <c r="C205" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -9466,7 +9449,7 @@
         <v>50</v>
       </c>
       <c r="C206" t="s">
-        <v>547</v>
+        <v>561</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -9477,7 +9460,7 @@
         <v>51</v>
       </c>
       <c r="C207" t="s">
-        <v>503</v>
+        <v>529</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -9488,7 +9471,7 @@
         <v>52</v>
       </c>
       <c r="C208" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -9499,7 +9482,7 @@
         <v>53</v>
       </c>
       <c r="C209" t="s">
-        <v>505</v>
+        <v>531</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -9510,7 +9493,7 @@
         <v>54</v>
       </c>
       <c r="C210" t="s">
-        <v>549</v>
+        <v>530</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -9521,7 +9504,7 @@
         <v>55</v>
       </c>
       <c r="C211" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -9532,7 +9515,7 @@
         <v>56</v>
       </c>
       <c r="C212" t="s">
-        <v>551</v>
+        <v>532</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -9543,7 +9526,7 @@
         <v>57</v>
       </c>
       <c r="C213" t="s">
-        <v>552</v>
+        <v>533</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -9554,7 +9537,7 @@
         <v>58</v>
       </c>
       <c r="C214" t="s">
-        <v>508</v>
+        <v>534</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -9565,7 +9548,7 @@
         <v>59</v>
       </c>
       <c r="C215" t="s">
-        <v>553</v>
+        <v>562</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -9576,7 +9559,7 @@
         <v>60</v>
       </c>
       <c r="C216" t="s">
-        <v>528</v>
+        <v>561</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -9587,7 +9570,7 @@
         <v>61</v>
       </c>
       <c r="C217" t="s">
-        <v>554</v>
+        <v>535</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -9598,7 +9581,7 @@
         <v>62</v>
       </c>
       <c r="C218" t="s">
-        <v>555</v>
+        <v>503</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -9609,7 +9592,7 @@
         <v>63</v>
       </c>
       <c r="C219" t="s">
-        <v>556</v>
+        <v>536</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -9620,7 +9603,7 @@
         <v>64</v>
       </c>
       <c r="C220" t="s">
-        <v>557</v>
+        <v>504</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -9631,7 +9614,7 @@
         <v>65</v>
       </c>
       <c r="C221" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -9642,7 +9625,7 @@
         <v>66</v>
       </c>
       <c r="C222" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -9653,7 +9636,7 @@
         <v>67</v>
       </c>
       <c r="C223" t="s">
-        <v>560</v>
+        <v>537</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -9664,7 +9647,7 @@
         <v>68</v>
       </c>
       <c r="C224" t="s">
-        <v>561</v>
+        <v>538</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -9675,7 +9658,7 @@
         <v>69</v>
       </c>
       <c r="C225" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -9686,7 +9669,7 @@
         <v>70</v>
       </c>
       <c r="C226" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -9697,7 +9680,7 @@
         <v>71</v>
       </c>
       <c r="C227" t="s">
-        <v>564</v>
+        <v>506</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -9708,7 +9691,7 @@
         <v>72</v>
       </c>
       <c r="C228" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -9719,7 +9702,7 @@
         <v>73</v>
       </c>
       <c r="C229" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -9730,7 +9713,7 @@
         <v>74</v>
       </c>
       <c r="C230" t="s">
-        <v>566</v>
+        <v>522</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -9741,7 +9724,7 @@
         <v>75</v>
       </c>
       <c r="C231" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -9752,7 +9735,7 @@
         <v>76</v>
       </c>
       <c r="C232" t="s">
-        <v>567</v>
+        <v>540</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -9763,7 +9746,7 @@
         <v>77</v>
       </c>
       <c r="C233" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -9774,7 +9757,7 @@
         <v>78</v>
       </c>
       <c r="C234" t="s">
-        <v>509</v>
+        <v>563</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -9785,7 +9768,7 @@
         <v>79</v>
       </c>
       <c r="C235" t="s">
-        <v>569</v>
+        <v>541</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -9796,7 +9779,7 @@
         <v>80</v>
       </c>
       <c r="C236" t="s">
-        <v>570</v>
+        <v>542</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -9807,7 +9790,7 @@
         <v>81</v>
       </c>
       <c r="C237" t="s">
-        <v>571</v>
+        <v>543</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -9818,7 +9801,7 @@
         <v>82</v>
       </c>
       <c r="C238" t="s">
-        <v>572</v>
+        <v>527</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -9829,7 +9812,7 @@
         <v>83</v>
       </c>
       <c r="C239" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -9840,7 +9823,7 @@
         <v>84</v>
       </c>
       <c r="C240" t="s">
-        <v>509</v>
+        <v>544</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -9851,7 +9834,7 @@
         <v>85</v>
       </c>
       <c r="C241" t="s">
-        <v>574</v>
+        <v>545</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -9862,7 +9845,7 @@
         <v>86</v>
       </c>
       <c r="C242" t="s">
-        <v>575</v>
+        <v>546</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -9873,7 +9856,7 @@
         <v>87</v>
       </c>
       <c r="C243" t="s">
-        <v>576</v>
+        <v>547</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -9884,15 +9867,240 @@
         <v>88</v>
       </c>
       <c r="C244" t="s">
-        <v>577</v>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B245" s="15">
+        <v>89</v>
+      </c>
+      <c r="C245" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B246" s="15">
+        <v>90</v>
+      </c>
+      <c r="C246" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B247" s="15">
+        <v>91</v>
+      </c>
+      <c r="C247" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B248" s="15">
+        <v>92</v>
+      </c>
+      <c r="C248" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B249" s="15">
+        <v>93</v>
+      </c>
+      <c r="C249" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B250" s="15">
+        <v>94</v>
+      </c>
+      <c r="C250" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B251" s="15">
+        <v>95</v>
+      </c>
+      <c r="C251" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B252" s="15">
+        <v>96</v>
+      </c>
+      <c r="C252" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B253" s="15">
+        <v>97</v>
+      </c>
+      <c r="C253" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B254" s="15">
+        <v>98</v>
+      </c>
+      <c r="C254" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B255" s="15">
+        <v>99</v>
+      </c>
+      <c r="C255" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B256" s="15">
+        <v>100</v>
+      </c>
+      <c r="C256" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B257" s="15">
+        <v>101</v>
+      </c>
+      <c r="C257" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B258" s="15">
+        <v>102</v>
+      </c>
+      <c r="C258" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B259" s="15">
+        <v>103</v>
+      </c>
+      <c r="C259" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B260" s="15">
+        <v>104</v>
+      </c>
+      <c r="C260" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B261" s="15">
+        <v>105</v>
+      </c>
+      <c r="C261" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B262" s="15">
+        <v>106</v>
+      </c>
+      <c r="C262" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B263" s="15">
+        <v>107</v>
+      </c>
+      <c r="C263" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B264" s="15">
+        <v>108</v>
+      </c>
+      <c r="C264" s="15" t="s">
+        <v>561</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H2000">
-    <cfRule type="expression" dxfId="98" priority="1">
+  <conditionalFormatting sqref="A265:H2019 A2:H106 C208:H211 C202:H206 C197:H200 C189:H195 C182:H187 C178:H180 C173:H176 C168:H171 C164:H166 C107:H162 C260:H264 C255:H258 C248:H253 C241:H246 C236:H239 C231:H234 C228:H229 C224:H226 C218:H222 C213:H216 A107:B264">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT($A2=$A1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C212:H212 C207:H207 C201:H201 C196:H196 C188:H188 C181:H181 C177:H177 C172:H172 C167:H167 C163:H163 C259:H259 C254:H254 C247:H247 C240:H240 C235:H235 C230:H230 C227:H227 C223:H223 C217:H217">
+    <cfRule type="expression" dxfId="99" priority="149">
+      <formula>NOT($A163=$A161)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -9949,7 +10157,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007061609</v>
+        <v>2007092010</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -13589,348 +13797,348 @@
     <mergeCell ref="A78:B78"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added next button movements
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA381FFC-DE3F-4D16-87D9-704732E96273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241E1668-B26F-4735-B602-44C46260B822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3935,6 +3935,745 @@
   </cellStyles>
   <dxfs count="232">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -3949,745 +4688,6 @@
           <color auto="1"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6123,8 +6123,8 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14:D17"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -10094,12 +10094,12 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A265:H2019 A2:H106 C208:H211 C202:H206 C197:H200 C189:H195 C182:H187 C178:H180 C173:H176 C168:H171 C164:H166 C107:H162 C260:H264 C255:H258 C248:H253 C241:H246 C236:H239 C231:H234 C228:H229 C224:H226 C218:H222 C213:H216 A107:B264">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="99" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C212:H212 C207:H207 C201:H201 C196:H196 C188:H188 C181:H181 C177:H177 C172:H172 C167:H167 C163:H163 C259:H259 C254:H254 C247:H247 C240:H240 C235:H235 C230:H230 C227:H227 C223:H223 C217:H217">
-    <cfRule type="expression" dxfId="99" priority="149">
+    <cfRule type="expression" dxfId="98" priority="149">
       <formula>NOT($A163=$A161)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007092010</v>
+        <v>2007131028</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -13797,348 +13797,348 @@
     <mergeCell ref="A78:B78"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="98" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="97" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="96" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="93" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="92" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="91" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="88" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="87" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="85" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="84" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="65" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="41" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="38" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added back button functionality.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241E1668-B26F-4735-B602-44C46260B822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BA8A66-3518-4C64-86DD-F36FA2E69674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -6124,7 +6124,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14:D16"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007131028</v>
+        <v>2007131745</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
updated number of rows implementation.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BA8A66-3518-4C64-86DD-F36FA2E69674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44439F7-DCB4-4DE2-9205-CE9319632547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6124,7 +6124,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15:D17"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007131745</v>
+        <v>2007131757</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
change workflow for large screen
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44439F7-DCB4-4DE2-9205-CE9319632547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D3BD68-5C6A-4272-B536-D3A3350E5D19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -6123,8 +6123,8 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15:D18"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -6363,6 +6363,9 @@
       <c r="C14" s="10" t="s">
         <v>368</v>
       </c>
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
       <c r="N14" s="9" t="s">
         <v>373</v>
       </c>
@@ -10157,7 +10160,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007131757</v>
+        <v>2007151223</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
update screen size parameter
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198E5BDA-7910-4D12-A372-EF3EC6FC5B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB236880-E7D4-43EF-B379-AACFBCC51CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,392 +3977,6 @@
   </cellStyles>
   <dxfs count="367">
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFEEB400"/>
@@ -5132,6 +4746,392 @@
           <color auto="1"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7187,8 +7187,8 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7431,7 +7431,7 @@
         <v>368</v>
       </c>
       <c r="D14" s="11">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>557</v>
@@ -7450,9 +7450,6 @@
       <c r="C15" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="D15" s="11">
-        <v>5</v>
-      </c>
       <c r="J15" s="9" t="s">
         <v>557</v>
       </c>
@@ -7487,9 +7484,6 @@
       <c r="C17" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="D17" s="11">
-        <v>4</v>
-      </c>
       <c r="J17" s="9" t="s">
         <v>557</v>
       </c>
@@ -7507,9 +7501,6 @@
       <c r="C18" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="D18" s="11">
-        <v>2</v>
-      </c>
       <c r="J18" s="9" t="s">
         <v>557</v>
       </c>
@@ -7682,9 +7673,6 @@
       </c>
       <c r="C28" s="10" t="s">
         <v>494</v>
-      </c>
-      <c r="D28" s="11">
-        <v>1</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>557</v>
@@ -8662,185 +8650,185 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="expression" dxfId="50" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="34" stopIfTrue="1">
       <formula>$A29="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="35" stopIfTrue="1">
       <formula>OR($A29="audio", $A29="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="36" stopIfTrue="1">
       <formula>$A29="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="37" stopIfTrue="1">
       <formula>OR($A29="date", $A29="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="38" stopIfTrue="1">
       <formula>OR($A29="calculate", $A29="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="39" stopIfTrue="1">
       <formula>$A29="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="40" stopIfTrue="1">
       <formula>$A29="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="41" stopIfTrue="1">
       <formula>OR($A29="geopoint", $A29="geoshape", $A29="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="42" stopIfTrue="1">
       <formula>OR($A29="audio audit", $A29="text audit", $A29="speed violations count", $A29="speed violations list", $A29="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="43" stopIfTrue="1">
       <formula>OR($A29="username", $A29="phonenumber", $A29="start", $A29="end", $A29="deviceid", $A29="subscriberid", $A29="simserial", $A29="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="44" stopIfTrue="1">
       <formula>OR(AND(LEFT($A29, 16)="select_multiple ", LEN($A29)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A29, 17)))), AND(LEFT($A29, 11)="select_one ", LEN($A29)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A29, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="45" stopIfTrue="1">
       <formula>$A29="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="46" stopIfTrue="1">
       <formula>$A29="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="47" stopIfTrue="1">
       <formula>$A29="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="48" stopIfTrue="1">
       <formula>$A29="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="49" stopIfTrue="1">
       <formula>$A29="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="50" stopIfTrue="1">
       <formula>$A29="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="51" stopIfTrue="1">
       <formula>$A29="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29 I29 F29">
-    <cfRule type="expression" dxfId="32" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="32" stopIfTrue="1">
       <formula>$A29="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29 O29 I29">
-    <cfRule type="expression" dxfId="31" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="29" stopIfTrue="1">
       <formula>$A29="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:D29 F29">
-    <cfRule type="expression" dxfId="30" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="26" stopIfTrue="1">
       <formula>$A29="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:D29 G29:H29">
-    <cfRule type="expression" dxfId="29" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="24" stopIfTrue="1">
       <formula>$A29="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:D29 G29:H29">
-    <cfRule type="expression" dxfId="28" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="22" stopIfTrue="1">
       <formula>$A29="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29 F29">
-    <cfRule type="expression" dxfId="27" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="20" stopIfTrue="1">
       <formula>OR(AND(LEFT($A29, 16)="select_multiple ", LEN($A29)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A29, 17)))), AND(LEFT($A29, 11)="select_one ", LEN($A29)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A29, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29 B29">
-    <cfRule type="expression" dxfId="26" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="17" stopIfTrue="1">
       <formula>OR($A29="audio audit", $A29="text audit", $A29="speed violations count", $A29="speed violations list", $A29="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="11" stopIfTrue="1">
       <formula>$A29="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="13" stopIfTrue="1">
       <formula>$A29="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="15" stopIfTrue="1">
       <formula>OR($A29="geopoint", $A29="geoshape", $A29="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29 N29">
-    <cfRule type="expression" dxfId="22" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="9" stopIfTrue="1">
       <formula>OR($A29="calculate", $A29="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29 F29">
-    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="7" stopIfTrue="1">
       <formula>OR($A29="date", $A29="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29 F29">
-    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="5" stopIfTrue="1">
       <formula>$A29="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="3" stopIfTrue="1">
       <formula>OR($A29="audio", $A29="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:I29 K29:W29">
-    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="2" stopIfTrue="1">
       <formula>$A29="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="4" stopIfTrue="1">
       <formula>OR($A29="audio", $A29="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="6" stopIfTrue="1">
       <formula>$A29="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="8" stopIfTrue="1">
       <formula>OR($A29="date", $A29="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="10" stopIfTrue="1">
       <formula>OR($A29="calculate", $A29="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="12" stopIfTrue="1">
       <formula>$A29="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="14" stopIfTrue="1">
       <formula>$A29="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="16" stopIfTrue="1">
       <formula>OR($A29="geopoint", $A29="geoshape", $A29="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="18" stopIfTrue="1">
       <formula>OR($A29="audio audit", $A29="text audit", $A29="speed violations count", $A29="speed violations list", $A29="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="19" stopIfTrue="1">
       <formula>OR($A29="username", $A29="phonenumber", $A29="start", $A29="end", $A29="deviceid", $A29="subscriberid", $A29="simserial", $A29="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="21" stopIfTrue="1">
       <formula>OR(AND(LEFT($A29, 16)="select_multiple ", LEN($A29)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A29, 17)))), AND(LEFT($A29, 11)="select_one ", LEN($A29)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A29, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="23" stopIfTrue="1">
       <formula>$A29="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="25" stopIfTrue="1">
       <formula>$A29="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="27" stopIfTrue="1">
       <formula>$A29="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="28" stopIfTrue="1">
       <formula>$A29="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="30" stopIfTrue="1">
       <formula>$A29="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="31" stopIfTrue="1">
       <formula>$A29="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="33" stopIfTrue="1">
       <formula>$A29="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
       <formula>$A29="comments"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11752,12 +11740,12 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A265:H2019 A2:H106 C208:H211 C202:H206 C197:H200 C189:H195 C182:H187 C178:H180 C173:H176 C168:H171 C164:H166 C107:H162 C260:H264 C255:H258 C248:H253 C241:H246 C236:H239 C231:H234 C228:H229 C224:H226 C218:H222 C213:H216 A107:B264">
-    <cfRule type="expression" dxfId="150" priority="1">
+    <cfRule type="expression" dxfId="99" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C212:H212 C207:H207 C201:H201 C196:H196 C188:H188 C181:H181 C177:H177 C172:H172 C167:H167 C163:H163 C259:H259 C254:H254 C247:H247 C240:H240 C235:H235 C230:H230 C227:H227 C223:H223 C217:H217">
-    <cfRule type="expression" dxfId="149" priority="149">
+    <cfRule type="expression" dxfId="98" priority="149">
       <formula>NOT($A163=$A161)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11815,7 +11803,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007151748</v>
+        <v>2007160856</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -15455,348 +15443,348 @@
     <mergeCell ref="A78:B78"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="148" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="147" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="146" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="145" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="144" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="143" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="142" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="141" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="138" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="137" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="136" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="135" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="134" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="116" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="115" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="97" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="96" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="95" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="94" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="91" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="90" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="89" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="88" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="87" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="86" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="68" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added double-clicking row number to select whole row.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB236880-E7D4-43EF-B379-AACFBCC51CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA11DA4-A851-47B3-AA65-E61455F64158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7187,8 +7187,8 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15:D18"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7450,6 +7450,9 @@
       <c r="C15" s="10" t="s">
         <v>369</v>
       </c>
+      <c r="D15" s="11">
+        <v>9</v>
+      </c>
       <c r="J15" s="9" t="s">
         <v>557</v>
       </c>
@@ -7467,6 +7470,9 @@
       <c r="C16" s="10" t="s">
         <v>370</v>
       </c>
+      <c r="D16" s="11">
+        <v>2</v>
+      </c>
       <c r="J16" s="9" t="s">
         <v>557</v>
       </c>
@@ -7603,6 +7609,9 @@
       <c r="C24" s="10" t="s">
         <v>369</v>
       </c>
+      <c r="D24" s="11">
+        <v>22</v>
+      </c>
       <c r="J24" s="9" t="s">
         <v>557</v>
       </c>
@@ -7619,6 +7628,9 @@
       </c>
       <c r="C25" s="10" t="s">
         <v>370</v>
+      </c>
+      <c r="D25" s="11">
+        <v>23</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>557</v>
@@ -11803,7 +11815,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007160856</v>
+        <v>2007161712</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
added different screen size view for passage and removed next button for small screens.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAF7AD2-16B2-4A1F-882E-DDCB73F3E1F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039B16C0-55F0-4B6E-ACBC-F910DCF49698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8994" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="587">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7187,8 +7187,8 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23:D27"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7416,9 +7416,6 @@
       <c r="F13" s="9" t="s">
         <v>559</v>
       </c>
-      <c r="J13" s="9" t="s">
-        <v>557</v>
-      </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="9" t="s">
@@ -7678,7 +7675,7 @@
         <v>494</v>
       </c>
       <c r="D28" s="11">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>557</v>
@@ -11809,7 +11806,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007171923</v>
+        <v>2007201044</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
removed full window reload.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039B16C0-55F0-4B6E-ACBC-F910DCF49698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD545124-A559-48AC-8322-676B23AB219C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7187,8 +7187,8 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7675,7 +7675,7 @@
         <v>494</v>
       </c>
       <c r="D28" s="11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>557</v>
@@ -7826,6 +7826,9 @@
       </c>
       <c r="C37" s="10" t="s">
         <v>480</v>
+      </c>
+      <c r="D37" s="11">
+        <v>4</v>
       </c>
       <c r="J37" s="9" t="s">
         <v>557</v>
@@ -11806,7 +11809,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007201044</v>
+        <v>2007201156</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
Update EGRA grid sample form.xlsx
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CA8A97-C5F4-4142-8FC6-619D0FBA1224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01531274-B7CA-420B-932B-F9E2BB000CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="593">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7207,7 +7207,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7433,7 +7433,9 @@
         <v>591</v>
       </c>
       <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="J13" s="11" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="9" t="s">
@@ -11828,7 +11830,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007291806</v>
+        <v>2007291807</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
added highlighting selected options on return to field.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01531274-B7CA-420B-932B-F9E2BB000CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC1D363-13BA-4757-B275-260904FDCE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7207,7 +7207,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7464,6 +7464,9 @@
       <c r="C15" s="10" t="s">
         <v>368</v>
       </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
       <c r="N15" s="9" t="s">
         <v>373</v>
       </c>
@@ -7477,6 +7480,9 @@
       </c>
       <c r="C16" s="10" t="s">
         <v>369</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2</v>
       </c>
       <c r="N16" s="9" t="s">
         <v>374</v>
@@ -11830,7 +11836,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007291807</v>
+        <v>2008041903</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -11978,7 +11984,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="39" customFormat="1" ht="187.2">
+    <row r="6" spans="1:30" s="39" customFormat="1" ht="202.8">
       <c r="A6" s="38" t="s">
         <v>278</v>
       </c>
@@ -12382,7 +12388,7 @@
       <c r="AC16" s="43"/>
       <c r="AD16" s="43"/>
     </row>
-    <row r="17" spans="1:30" s="45" customFormat="1" ht="31.2">
+    <row r="17" spans="1:30" s="45" customFormat="1" ht="46.8">
       <c r="A17" s="43" t="s">
         <v>103</v>
       </c>
@@ -15978,7 +15984,7 @@
       </c>
       <c r="H5" s="35"/>
     </row>
-    <row r="6" spans="1:8" s="39" customFormat="1" ht="296.39999999999998">
+    <row r="6" spans="1:8" s="39" customFormat="1" ht="312">
       <c r="A6" s="38" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
added preserving state when returning to field.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC1D363-13BA-4757-B275-260904FDCE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96AB79-6AFB-4F9B-ACEB-8DDF7E52F57A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7207,7 +7207,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7498,6 +7498,9 @@
       <c r="C17" s="10" t="s">
         <v>370</v>
       </c>
+      <c r="D17" s="11">
+        <v>3</v>
+      </c>
       <c r="N17" s="9" t="s">
         <v>375</v>
       </c>
@@ -7512,6 +7515,9 @@
       <c r="C18" s="10" t="s">
         <v>371</v>
       </c>
+      <c r="D18" s="11">
+        <v>4</v>
+      </c>
       <c r="N18" s="9" t="s">
         <v>376</v>
       </c>
@@ -7525,6 +7531,9 @@
       </c>
       <c r="C19" s="10" t="s">
         <v>372</v>
+      </c>
+      <c r="D19" s="11">
+        <v>5</v>
       </c>
       <c r="N19" s="9" t="s">
         <v>377</v>
@@ -11836,7 +11845,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008041903</v>
+        <v>2008051806</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -11984,7 +11993,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="39" customFormat="1" ht="202.8">
+    <row r="6" spans="1:30" s="39" customFormat="1" ht="187.2">
       <c r="A6" s="38" t="s">
         <v>278</v>
       </c>
@@ -12388,7 +12397,7 @@
       <c r="AC16" s="43"/>
       <c r="AD16" s="43"/>
     </row>
-    <row r="17" spans="1:30" s="45" customFormat="1" ht="46.8">
+    <row r="17" spans="1:30" s="45" customFormat="1" ht="31.2">
       <c r="A17" s="43" t="s">
         <v>103</v>
       </c>
@@ -15984,7 +15993,7 @@
       </c>
       <c r="H5" s="35"/>
     </row>
-    <row r="6" spans="1:8" s="39" customFormat="1" ht="312">
+    <row r="6" spans="1:8" s="39" customFormat="1" ht="296.39999999999998">
       <c r="A6" s="38" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
added continue timer on paging back functionality.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96AB79-6AFB-4F9B-ACEB-8DDF7E52F57A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F24A2A2-E066-4BE7-BE92-8056A820B6B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="596">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3276,9 +3276,6 @@
 Whether the firstline was completed or not ${endFirstLine}</t>
   </si>
   <si>
-    <t>custom-egra-grid(type='reading', duration='20', pause=0, strict=1)</t>
-  </si>
-  <si>
     <t>advance</t>
   </si>
   <si>
@@ -3286,6 +3283,18 @@
   </si>
   <si>
     <t>Click/tap the button to start.</t>
+  </si>
+  <si>
+    <t>custom-egra-grid(type='reading', duration='20', pause=1, strict=1)</t>
+  </si>
+  <si>
+    <t>item-at('|', plug-in-metadata(${letters}), 6)</t>
+  </si>
+  <si>
+    <t>item-at('|', plug-in-metadata(${letters}), 7)</t>
+  </si>
+  <si>
+    <t>item-at('|', plug-in-metadata(${letters}), 8)</t>
   </si>
 </sst>
 </file>
@@ -7206,8 +7215,8 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7424,13 +7433,13 @@
         <v>97</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>590</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>592</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>591</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11" t="s">
@@ -7451,7 +7460,7 @@
         <v>380</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -7465,10 +7474,10 @@
         <v>368</v>
       </c>
       <c r="D15" s="11">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -7482,10 +7491,10 @@
         <v>369</v>
       </c>
       <c r="D16" s="11">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -7499,10 +7508,10 @@
         <v>370</v>
       </c>
       <c r="D17" s="11">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>375</v>
+        <v>587</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -7516,10 +7525,10 @@
         <v>371</v>
       </c>
       <c r="D18" s="11">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>376</v>
+        <v>593</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="31.2">
@@ -7533,10 +7542,10 @@
         <v>372</v>
       </c>
       <c r="D19" s="11">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>377</v>
+        <v>594</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -7549,8 +7558,11 @@
       <c r="C20" s="10" t="s">
         <v>586</v>
       </c>
+      <c r="D20" s="11">
+        <v>49</v>
+      </c>
       <c r="N20" s="9" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="156">
@@ -7562,6 +7574,9 @@
       </c>
       <c r="C21" s="10" t="s">
         <v>588</v>
+      </c>
+      <c r="D21" s="11">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="31.2">
@@ -11845,7 +11860,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008051806</v>
+        <v>2008061632</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
added double confirmong finished button.
</commit_message>
<xml_diff>
--- a/source/EGRA grid sample form.xlsx
+++ b/source/EGRA grid sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\egra-grid\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97F79DB-439B-4C55-BEA4-766E848B90D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDECDD27-C878-42E6-8A71-9E08FF71BE5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7216,7 +7216,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7542,7 +7542,7 @@
         <v>372</v>
       </c>
       <c r="D19" s="11">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="N19" s="9" t="s">
         <v>587</v>
@@ -7559,7 +7559,7 @@
         <v>580</v>
       </c>
       <c r="D20" s="11">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="N20" s="9" t="s">
         <v>588</v>
@@ -11860,7 +11860,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008071520</v>
+        <v>2008071622</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>